<commit_message>
Corrected OOI Bar Code numbers
</commit_message>
<xml_diff>
--- a/deployment/Omaha_Cal_Info_CE01ISSM_00005.xlsx
+++ b/deployment/Omaha_Cal_Info_CE01ISSM_00005.xlsx
@@ -596,13 +596,7 @@
     <t>OL000291</t>
   </si>
   <si>
-    <t>OL000272</t>
-  </si>
-  <si>
     <t>CE01ISSM-00005-MOPAK</t>
-  </si>
-  <si>
-    <t>OL000273</t>
   </si>
   <si>
     <t>N00420</t>
@@ -635,9 +629,6 @@
     <t>A00056</t>
   </si>
   <si>
-    <t>OL000274</t>
-  </si>
-  <si>
     <t>A00174</t>
   </si>
   <si>
@@ -656,13 +647,22 @@
     <t>A01151</t>
   </si>
   <si>
-    <t>OL000275</t>
+    <t>OL000292</t>
   </si>
   <si>
-    <t>OL000276</t>
+    <t>OL000293</t>
   </si>
   <si>
-    <t>OL000277</t>
+    <t>OL000294</t>
+  </si>
+  <si>
+    <t>OL000295</t>
+  </si>
+  <si>
+    <t>OL000296</t>
+  </si>
+  <si>
+    <t>OL000297</t>
   </si>
 </sst>
 </file>
@@ -867,7 +867,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="15">
+  <fills count="16">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -948,6 +948,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1194,7 +1200,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1361,6 +1367,7 @@
     <xf numFmtId="0" fontId="7" fillId="14" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="166">
     <cellStyle name="Comma" xfId="2" builtinId="3"/>
@@ -2019,8 +2026,8 @@
   <dimension ref="A1:AMM225"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A21" sqref="A21"/>
+      <pane ySplit="1" topLeftCell="A197" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E229" sqref="E229"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3787,11 +3794,11 @@
       <c r="D39" s="8">
         <v>5</v>
       </c>
-      <c r="E39" t="s">
+      <c r="E39" s="60" t="s">
+        <v>206</v>
+      </c>
+      <c r="F39" t="s">
         <v>189</v>
-      </c>
-      <c r="F39" t="s">
-        <v>190</v>
       </c>
       <c r="G39" s="10" t="s">
         <v>17</v>
@@ -5855,7 +5862,7 @@
         <v>5</v>
       </c>
       <c r="E41" t="s">
-        <v>191</v>
+        <v>207</v>
       </c>
       <c r="F41" s="28" t="s">
         <v>155</v>
@@ -6897,7 +6904,7 @@
         <v>5</v>
       </c>
       <c r="E42" t="s">
-        <v>191</v>
+        <v>207</v>
       </c>
       <c r="F42" s="28" t="s">
         <v>155</v>
@@ -8967,7 +8974,7 @@
         <v>5</v>
       </c>
       <c r="E44" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="F44" s="25" t="s">
         <v>156</v>
@@ -8994,7 +9001,7 @@
         <v>5</v>
       </c>
       <c r="E45" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="F45" s="25" t="s">
         <v>156</v>
@@ -9021,7 +9028,7 @@
         <v>5</v>
       </c>
       <c r="E46" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="F46" s="25" t="s">
         <v>156</v>
@@ -9047,7 +9054,7 @@
         <v>5</v>
       </c>
       <c r="E47" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="F47" s="25" t="s">
         <v>156</v>
@@ -9073,7 +9080,7 @@
         <v>5</v>
       </c>
       <c r="E48" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="F48" s="25" t="s">
         <v>156</v>
@@ -9099,7 +9106,7 @@
         <v>5</v>
       </c>
       <c r="E49" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="F49" s="25" t="s">
         <v>156</v>
@@ -9125,7 +9132,7 @@
         <v>5</v>
       </c>
       <c r="E50" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="F50" s="25" t="s">
         <v>156</v>
@@ -9151,7 +9158,7 @@
         <v>5</v>
       </c>
       <c r="E51" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="F51" s="25" t="s">
         <v>156</v>
@@ -9177,7 +9184,7 @@
         <v>5</v>
       </c>
       <c r="E52" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="F52" s="25" t="s">
         <v>156</v>
@@ -9203,7 +9210,7 @@
         <v>5</v>
       </c>
       <c r="E53" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="F53" s="25" t="s">
         <v>156</v>
@@ -9229,7 +9236,7 @@
         <v>5</v>
       </c>
       <c r="E54" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="F54" s="25" t="s">
         <v>156</v>
@@ -9255,7 +9262,7 @@
         <v>5</v>
       </c>
       <c r="E55" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="F55" s="25" t="s">
         <v>156</v>
@@ -9281,7 +9288,7 @@
         <v>5</v>
       </c>
       <c r="E56" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="F56" s="25" t="s">
         <v>156</v>
@@ -9307,7 +9314,7 @@
         <v>5</v>
       </c>
       <c r="E57" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="F57" s="25" t="s">
         <v>156</v>
@@ -9333,7 +9340,7 @@
         <v>5</v>
       </c>
       <c r="E58" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="F58" s="25" t="s">
         <v>156</v>
@@ -9359,7 +9366,7 @@
         <v>5</v>
       </c>
       <c r="E59" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="F59" s="25" t="s">
         <v>156</v>
@@ -9385,7 +9392,7 @@
         <v>5</v>
       </c>
       <c r="E60" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="F60" s="25" t="s">
         <v>156</v>
@@ -9411,7 +9418,7 @@
         <v>5</v>
       </c>
       <c r="E61" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="F61" s="25" t="s">
         <v>156</v>
@@ -9437,7 +9444,7 @@
         <v>5</v>
       </c>
       <c r="E62" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="F62" s="25" t="s">
         <v>156</v>
@@ -9463,7 +9470,7 @@
         <v>5</v>
       </c>
       <c r="E63" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="F63" s="25" t="s">
         <v>156</v>
@@ -9489,7 +9496,7 @@
         <v>5</v>
       </c>
       <c r="E64" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="F64" s="25" t="s">
         <v>156</v>
@@ -9515,7 +9522,7 @@
         <v>5</v>
       </c>
       <c r="E65" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="F65" s="25" t="s">
         <v>156</v>
@@ -9541,7 +9548,7 @@
         <v>5</v>
       </c>
       <c r="E66" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="F66" s="25" t="s">
         <v>156</v>
@@ -9567,7 +9574,7 @@
         <v>5</v>
       </c>
       <c r="E67" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="F67" s="25" t="s">
         <v>156</v>
@@ -9604,7 +9611,7 @@
         <v>5</v>
       </c>
       <c r="E69" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="F69" s="25">
         <v>218</v>
@@ -9631,7 +9638,7 @@
         <v>5</v>
       </c>
       <c r="E70" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="F70" s="25">
         <v>218</v>
@@ -9658,7 +9665,7 @@
         <v>5</v>
       </c>
       <c r="E71" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="F71" s="25">
         <v>218</v>
@@ -9685,7 +9692,7 @@
         <v>5</v>
       </c>
       <c r="E72" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="F72" s="25">
         <v>218</v>
@@ -10743,7 +10750,7 @@
         <v>5</v>
       </c>
       <c r="E74" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="F74" s="25">
         <v>995</v>
@@ -10770,7 +10777,7 @@
         <v>5</v>
       </c>
       <c r="E75" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="F75" s="25">
         <v>995</v>
@@ -10797,7 +10804,7 @@
         <v>5</v>
       </c>
       <c r="E76" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="F76" s="25">
         <v>995</v>
@@ -10824,7 +10831,7 @@
         <v>5</v>
       </c>
       <c r="E77" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="F77" s="25">
         <v>995</v>
@@ -10851,7 +10858,7 @@
         <v>5</v>
       </c>
       <c r="E78" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="F78" s="25">
         <v>995</v>
@@ -10878,7 +10885,7 @@
         <v>5</v>
       </c>
       <c r="E79" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="F79" s="25">
         <v>995</v>
@@ -10905,7 +10912,7 @@
         <v>5</v>
       </c>
       <c r="E80" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="F80" s="25">
         <v>995</v>
@@ -10934,7 +10941,7 @@
         <v>5</v>
       </c>
       <c r="E81" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="F81" s="25">
         <v>995</v>
@@ -10963,7 +10970,7 @@
         <v>5</v>
       </c>
       <c r="E82" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="F82" s="25">
         <v>995</v>
@@ -10992,7 +10999,7 @@
         <v>5</v>
       </c>
       <c r="E83" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="F83" s="25">
         <v>995</v>
@@ -11032,7 +11039,7 @@
         <v>5</v>
       </c>
       <c r="E85" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="F85" s="25">
         <v>263</v>
@@ -11061,7 +11068,7 @@
         <v>5</v>
       </c>
       <c r="E86" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="F86" s="25">
         <v>263</v>
@@ -11090,7 +11097,7 @@
         <v>5</v>
       </c>
       <c r="E87" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="F87" s="25">
         <v>263</v>
@@ -11117,7 +11124,7 @@
         <v>5</v>
       </c>
       <c r="E88" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="F88" s="25">
         <v>263</v>
@@ -11144,7 +11151,7 @@
         <v>5</v>
       </c>
       <c r="E89" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="F89" s="25">
         <v>263</v>
@@ -11171,7 +11178,7 @@
         <v>5</v>
       </c>
       <c r="E90" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="F90" s="25">
         <v>263</v>
@@ -11198,7 +11205,7 @@
         <v>5</v>
       </c>
       <c r="E91" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="F91" s="25">
         <v>263</v>
@@ -11236,7 +11243,7 @@
         <v>5</v>
       </c>
       <c r="E93" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="F93" s="28" t="s">
         <v>171</v>
@@ -12279,7 +12286,7 @@
         <v>5</v>
       </c>
       <c r="E94" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="F94" s="28" t="s">
         <v>171</v>
@@ -13323,7 +13330,7 @@
         <v>5</v>
       </c>
       <c r="E95" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="F95" s="28" t="s">
         <v>171</v>
@@ -14367,7 +14374,7 @@
         <v>5</v>
       </c>
       <c r="E96" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="F96" s="28" t="s">
         <v>171</v>
@@ -15411,7 +15418,7 @@
         <v>5</v>
       </c>
       <c r="E97" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="F97" s="28" t="s">
         <v>171</v>
@@ -16455,7 +16462,7 @@
         <v>5</v>
       </c>
       <c r="E98" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="F98" s="28" t="s">
         <v>171</v>
@@ -17499,7 +17506,7 @@
         <v>5</v>
       </c>
       <c r="E99" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="F99" s="28" t="s">
         <v>171</v>
@@ -18543,7 +18550,7 @@
         <v>5</v>
       </c>
       <c r="E100" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="F100" s="28" t="s">
         <v>171</v>
@@ -18581,7 +18588,7 @@
         <v>5</v>
       </c>
       <c r="E102" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="F102" s="25" t="s">
         <v>172</v>
@@ -18608,7 +18615,7 @@
         <v>5</v>
       </c>
       <c r="E103" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="F103" s="25" t="s">
         <v>172</v>
@@ -18635,7 +18642,7 @@
         <v>5</v>
       </c>
       <c r="E104" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="F104" s="25" t="s">
         <v>172</v>
@@ -18662,7 +18669,7 @@
         <v>5</v>
       </c>
       <c r="E105" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="F105" s="25" t="s">
         <v>172</v>
@@ -18689,7 +18696,7 @@
         <v>5</v>
       </c>
       <c r="E106" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="F106" s="25" t="s">
         <v>172</v>
@@ -18718,7 +18725,7 @@
         <v>5</v>
       </c>
       <c r="E107" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="F107" s="25" t="s">
         <v>172</v>
@@ -18747,7 +18754,7 @@
         <v>5</v>
       </c>
       <c r="E108" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="F108" s="25" t="s">
         <v>172</v>
@@ -18774,7 +18781,7 @@
         <v>5</v>
       </c>
       <c r="E109" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="F109" s="25" t="s">
         <v>172</v>
@@ -18812,7 +18819,7 @@
         <v>5</v>
       </c>
       <c r="E111" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="F111" s="25" t="s">
         <v>173</v>
@@ -19855,7 +19862,7 @@
         <v>5</v>
       </c>
       <c r="E112" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="F112" s="25" t="s">
         <v>173</v>
@@ -20898,7 +20905,7 @@
         <v>5</v>
       </c>
       <c r="E113" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="F113" s="25" t="s">
         <v>173</v>
@@ -21941,7 +21948,7 @@
         <v>5</v>
       </c>
       <c r="E114" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="F114" s="25" t="s">
         <v>173</v>
@@ -22984,7 +22991,7 @@
         <v>5</v>
       </c>
       <c r="E115" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="F115" s="25" t="s">
         <v>173</v>
@@ -24027,7 +24034,7 @@
         <v>5</v>
       </c>
       <c r="E116" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="F116" s="25" t="s">
         <v>173</v>
@@ -25070,7 +25077,7 @@
         <v>5</v>
       </c>
       <c r="E117" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="F117" s="55" t="s">
         <v>173</v>
@@ -27142,7 +27149,7 @@
         <v>5</v>
       </c>
       <c r="E119" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="F119" s="25">
         <v>250</v>
@@ -27169,7 +27176,7 @@
         <v>5</v>
       </c>
       <c r="E120" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="F120" s="25">
         <v>250</v>
@@ -27196,7 +27203,7 @@
         <v>5</v>
       </c>
       <c r="E121" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="F121" s="25">
         <v>250</v>
@@ -27234,7 +27241,7 @@
         <v>5</v>
       </c>
       <c r="E123" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="F123" s="25">
         <v>8535</v>
@@ -28278,7 +28285,7 @@
         <v>5</v>
       </c>
       <c r="E124" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="F124" s="25">
         <v>8535</v>
@@ -30349,7 +30356,7 @@
         <v>5</v>
       </c>
       <c r="E126" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="F126" s="41">
         <v>18225</v>
@@ -30378,7 +30385,7 @@
         <v>5</v>
       </c>
       <c r="E127" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="F127" s="25">
         <v>18225</v>
@@ -30405,7 +30412,7 @@
         <v>5</v>
       </c>
       <c r="E128" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="F128" s="25">
         <v>18225</v>
@@ -30432,7 +30439,7 @@
         <v>5</v>
       </c>
       <c r="E129" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="F129" s="25">
         <v>18225</v>
@@ -30459,7 +30466,7 @@
         <v>5</v>
       </c>
       <c r="E130" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="F130" s="25">
         <v>18225</v>
@@ -30486,7 +30493,7 @@
         <v>5</v>
       </c>
       <c r="E131" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="F131" s="25">
         <v>18225</v>
@@ -30513,7 +30520,7 @@
         <v>5</v>
       </c>
       <c r="E132" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="F132" s="25">
         <v>18225</v>
@@ -32600,7 +32607,7 @@
         <v>5</v>
       </c>
       <c r="E136" t="s">
-        <v>202</v>
+        <v>208</v>
       </c>
       <c r="F136" s="25" t="s">
         <v>176</v>
@@ -32626,7 +32633,7 @@
         <v>5</v>
       </c>
       <c r="E137" t="s">
-        <v>202</v>
+        <v>208</v>
       </c>
       <c r="F137" s="25" t="s">
         <v>176</v>
@@ -32652,7 +32659,7 @@
         <v>5</v>
       </c>
       <c r="E138" t="s">
-        <v>202</v>
+        <v>208</v>
       </c>
       <c r="F138" s="25" t="s">
         <v>176</v>
@@ -32678,7 +32685,7 @@
         <v>5</v>
       </c>
       <c r="E139" t="s">
-        <v>202</v>
+        <v>208</v>
       </c>
       <c r="F139" s="25" t="s">
         <v>176</v>
@@ -32704,7 +32711,7 @@
         <v>5</v>
       </c>
       <c r="E140" t="s">
-        <v>202</v>
+        <v>208</v>
       </c>
       <c r="F140" s="25" t="s">
         <v>176</v>
@@ -32730,7 +32737,7 @@
         <v>5</v>
       </c>
       <c r="E141" t="s">
-        <v>202</v>
+        <v>208</v>
       </c>
       <c r="F141" s="25" t="s">
         <v>176</v>
@@ -32756,7 +32763,7 @@
         <v>5</v>
       </c>
       <c r="E142" t="s">
-        <v>202</v>
+        <v>208</v>
       </c>
       <c r="F142" s="25" t="s">
         <v>176</v>
@@ -32782,7 +32789,7 @@
         <v>5</v>
       </c>
       <c r="E143" t="s">
-        <v>202</v>
+        <v>208</v>
       </c>
       <c r="F143" s="25" t="s">
         <v>176</v>
@@ -32808,7 +32815,7 @@
         <v>5</v>
       </c>
       <c r="E144" t="s">
-        <v>202</v>
+        <v>208</v>
       </c>
       <c r="F144" s="25" t="s">
         <v>176</v>
@@ -32834,7 +32841,7 @@
         <v>5</v>
       </c>
       <c r="E145" t="s">
-        <v>202</v>
+        <v>208</v>
       </c>
       <c r="F145" s="25" t="s">
         <v>176</v>
@@ -32860,7 +32867,7 @@
         <v>5</v>
       </c>
       <c r="E146" t="s">
-        <v>202</v>
+        <v>208</v>
       </c>
       <c r="F146" s="25" t="s">
         <v>176</v>
@@ -32886,7 +32893,7 @@
         <v>5</v>
       </c>
       <c r="E147" t="s">
-        <v>202</v>
+        <v>208</v>
       </c>
       <c r="F147" s="25" t="s">
         <v>176</v>
@@ -32912,7 +32919,7 @@
         <v>5</v>
       </c>
       <c r="E148" t="s">
-        <v>202</v>
+        <v>208</v>
       </c>
       <c r="F148" s="25" t="s">
         <v>176</v>
@@ -32938,7 +32945,7 @@
         <v>5</v>
       </c>
       <c r="E149" t="s">
-        <v>202</v>
+        <v>208</v>
       </c>
       <c r="F149" s="25" t="s">
         <v>176</v>
@@ -32964,7 +32971,7 @@
         <v>5</v>
       </c>
       <c r="E150" t="s">
-        <v>202</v>
+        <v>208</v>
       </c>
       <c r="F150" s="25" t="s">
         <v>176</v>
@@ -32990,7 +32997,7 @@
         <v>5</v>
       </c>
       <c r="E151" t="s">
-        <v>202</v>
+        <v>208</v>
       </c>
       <c r="F151" s="25" t="s">
         <v>176</v>
@@ -33016,7 +33023,7 @@
         <v>5</v>
       </c>
       <c r="E152" t="s">
-        <v>202</v>
+        <v>208</v>
       </c>
       <c r="F152" s="25" t="s">
         <v>176</v>
@@ -33042,7 +33049,7 @@
         <v>5</v>
       </c>
       <c r="E153" t="s">
-        <v>202</v>
+        <v>208</v>
       </c>
       <c r="F153" s="25" t="s">
         <v>176</v>
@@ -33068,7 +33075,7 @@
         <v>5</v>
       </c>
       <c r="E154" t="s">
-        <v>202</v>
+        <v>208</v>
       </c>
       <c r="F154" s="25" t="s">
         <v>176</v>
@@ -33094,7 +33101,7 @@
         <v>5</v>
       </c>
       <c r="E155" t="s">
-        <v>202</v>
+        <v>208</v>
       </c>
       <c r="F155" s="25" t="s">
         <v>176</v>
@@ -33120,7 +33127,7 @@
         <v>5</v>
       </c>
       <c r="E156" t="s">
-        <v>202</v>
+        <v>208</v>
       </c>
       <c r="F156" s="25" t="s">
         <v>176</v>
@@ -33146,7 +33153,7 @@
         <v>5</v>
       </c>
       <c r="E157" t="s">
-        <v>202</v>
+        <v>208</v>
       </c>
       <c r="F157" s="25" t="s">
         <v>176</v>
@@ -33172,7 +33179,7 @@
         <v>5</v>
       </c>
       <c r="E158" t="s">
-        <v>202</v>
+        <v>208</v>
       </c>
       <c r="F158" s="25" t="s">
         <v>176</v>
@@ -33198,7 +33205,7 @@
         <v>5</v>
       </c>
       <c r="E159" t="s">
-        <v>202</v>
+        <v>208</v>
       </c>
       <c r="F159" s="25" t="s">
         <v>176</v>
@@ -33235,7 +33242,7 @@
         <v>5</v>
       </c>
       <c r="E161" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="F161" s="25">
         <v>136</v>
@@ -33262,7 +33269,7 @@
         <v>5</v>
       </c>
       <c r="E162" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="F162" s="25">
         <v>136</v>
@@ -33289,7 +33296,7 @@
         <v>5</v>
       </c>
       <c r="E163" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="F163" s="25">
         <v>136</v>
@@ -33316,7 +33323,7 @@
         <v>5</v>
       </c>
       <c r="E164" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="F164" s="25">
         <v>136</v>
@@ -34546,7 +34553,7 @@
         <v>5</v>
       </c>
       <c r="E175" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="F175" s="26" t="s">
         <v>179</v>
@@ -34573,7 +34580,7 @@
         <v>5</v>
       </c>
       <c r="E176" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="F176" s="26" t="s">
         <v>179</v>
@@ -34600,7 +34607,7 @@
         <v>5</v>
       </c>
       <c r="E177" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="F177" s="26" t="s">
         <v>179</v>
@@ -34627,7 +34634,7 @@
         <v>5</v>
       </c>
       <c r="E178" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="F178" s="26" t="s">
         <v>179</v>
@@ -34654,7 +34661,7 @@
         <v>5</v>
       </c>
       <c r="E179" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="F179" s="26" t="s">
         <v>179</v>
@@ -34683,7 +34690,7 @@
         <v>5</v>
       </c>
       <c r="E180" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="F180" s="26" t="s">
         <v>179</v>
@@ -34712,7 +34719,7 @@
         <v>5</v>
       </c>
       <c r="E181" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="F181" s="26" t="s">
         <v>179</v>
@@ -34739,7 +34746,7 @@
         <v>5</v>
       </c>
       <c r="E182" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="F182" s="26" t="s">
         <v>179</v>
@@ -34776,7 +34783,7 @@
         <v>5</v>
       </c>
       <c r="E184" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="F184" s="25" t="s">
         <v>180</v>
@@ -35814,7 +35821,7 @@
         <v>5</v>
       </c>
       <c r="E185" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="F185" s="25" t="s">
         <v>180</v>
@@ -36852,7 +36859,7 @@
         <v>5</v>
       </c>
       <c r="E186" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="F186" s="25" t="s">
         <v>180</v>
@@ -37890,7 +37897,7 @@
         <v>5</v>
       </c>
       <c r="E187" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="F187" s="25" t="s">
         <v>180</v>
@@ -38928,7 +38935,7 @@
         <v>5</v>
       </c>
       <c r="E188" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="F188" s="25" t="s">
         <v>180</v>
@@ -39966,7 +39973,7 @@
         <v>5</v>
       </c>
       <c r="E189" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="F189" s="25" t="s">
         <v>180</v>
@@ -41004,7 +41011,7 @@
         <v>5</v>
       </c>
       <c r="E190" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="F190" s="56" t="s">
         <v>180</v>
@@ -42062,7 +42069,7 @@
         <v>5</v>
       </c>
       <c r="E192" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="F192" s="28" t="s">
         <v>181</v>
@@ -42091,7 +42098,7 @@
         <v>5</v>
       </c>
       <c r="E193" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="F193" s="28" t="s">
         <v>181</v>
@@ -42120,7 +42127,7 @@
         <v>5</v>
       </c>
       <c r="E194" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="F194" s="28" t="s">
         <v>181</v>
@@ -42147,7 +42154,7 @@
         <v>5</v>
       </c>
       <c r="E195" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="F195" s="28" t="s">
         <v>181</v>
@@ -42174,7 +42181,7 @@
         <v>5</v>
       </c>
       <c r="E196" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="F196" s="28" t="s">
         <v>181</v>
@@ -42201,7 +42208,7 @@
         <v>5</v>
       </c>
       <c r="E197" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="F197" s="28" t="s">
         <v>181</v>
@@ -42230,7 +42237,7 @@
         <v>5</v>
       </c>
       <c r="E198" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="F198" s="28" t="s">
         <v>181</v>
@@ -42259,7 +42266,7 @@
         <v>5</v>
       </c>
       <c r="E199" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="F199" s="28" t="s">
         <v>181</v>
@@ -42288,7 +42295,7 @@
         <v>5</v>
       </c>
       <c r="E200" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="F200" s="28" t="s">
         <v>181</v>
@@ -42315,7 +42322,7 @@
         <v>5</v>
       </c>
       <c r="E201" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="F201" s="28" t="s">
         <v>181</v>
@@ -42342,7 +42349,7 @@
         <v>5</v>
       </c>
       <c r="E202" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="F202" s="28" t="s">
         <v>181</v>
@@ -42369,7 +42376,7 @@
         <v>5</v>
       </c>
       <c r="E203" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="F203" s="28" t="s">
         <v>181</v>
@@ -42396,7 +42403,7 @@
         <v>5</v>
       </c>
       <c r="E204" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="F204" s="28" t="s">
         <v>181</v>
@@ -42423,7 +42430,7 @@
         <v>5</v>
       </c>
       <c r="E205" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="F205" s="28" t="s">
         <v>181</v>
@@ -42450,7 +42457,7 @@
         <v>5</v>
       </c>
       <c r="E206" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="F206" s="28" t="s">
         <v>181</v>
@@ -42477,7 +42484,7 @@
         <v>5</v>
       </c>
       <c r="E207" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="F207" s="28" t="s">
         <v>181</v>
@@ -42504,7 +42511,7 @@
         <v>5</v>
       </c>
       <c r="E208" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="F208" s="28" t="s">
         <v>181</v>
@@ -42531,7 +42538,7 @@
         <v>5</v>
       </c>
       <c r="E209" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="F209" s="28" t="s">
         <v>181</v>
@@ -42569,7 +42576,7 @@
         <v>5</v>
       </c>
       <c r="E211" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="F211" s="25">
         <v>11707</v>
@@ -42596,7 +42603,7 @@
         <v>5</v>
       </c>
       <c r="E212" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="F212" s="25">
         <v>11707</v>
@@ -42634,7 +42641,7 @@
         <v>5</v>
       </c>
       <c r="E214" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="F214" s="20">
         <v>55075</v>

</xml_diff>